<commit_message>
new analyses, paper write-up
</commit_message>
<xml_diff>
--- a/FiveYrRev/summary.xlsx
+++ b/FiveYrRev/summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="9510" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4514,6 +4514,1117 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Timeline of Recovery</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Plans with Recovery Units</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet6!$I$8:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$J$8:$J$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="256189096"/>
+        <c:axId val="256189880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="256189096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="256189880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="256189880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of Recovery Plans</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="256189096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4781,7 +5892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -28448,10 +29559,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28459,7 +29570,7 @@
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>397</v>
       </c>
@@ -28470,7 +29581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>398</v>
       </c>
@@ -28481,7 +29592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>410</v>
       </c>
@@ -28492,7 +29603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>425</v>
       </c>
@@ -28503,7 +29614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>453</v>
       </c>
@@ -28514,7 +29625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>460</v>
       </c>
@@ -28522,7 +29633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>500</v>
       </c>
@@ -28533,7 +29644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>510</v>
       </c>
@@ -28543,24 +29654,42 @@
       <c r="C8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1995</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>512</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1996</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>512</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1997</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -28570,8 +29699,14 @@
       <c r="C11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1998</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>539</v>
       </c>
@@ -28581,8 +29716,14 @@
       <c r="C12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1999</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>553</v>
       </c>
@@ -28592,8 +29733,14 @@
       <c r="C13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2000</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>562</v>
       </c>
@@ -28603,8 +29750,14 @@
       <c r="C14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>2001</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>573</v>
       </c>
@@ -28614,8 +29767,14 @@
       <c r="C15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>2002</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>576</v>
       </c>
@@ -28625,8 +29784,14 @@
       <c r="C16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>2003</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>585</v>
       </c>
@@ -28636,8 +29801,14 @@
       <c r="C17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>2004</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>167</v>
       </c>
@@ -28647,8 +29818,14 @@
       <c r="C18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>2005</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>594</v>
       </c>
@@ -28658,8 +29835,14 @@
       <c r="C19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>2006</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>600</v>
       </c>
@@ -28669,8 +29852,14 @@
       <c r="C20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>2007</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>185</v>
       </c>
@@ -28680,8 +29869,14 @@
       <c r="C21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>2008</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -28691,8 +29886,14 @@
       <c r="C22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>2009</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>608</v>
       </c>
@@ -28702,8 +29903,14 @@
       <c r="C23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>2010</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>644</v>
       </c>
@@ -28713,8 +29920,14 @@
       <c r="C24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>2011</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>649</v>
       </c>
@@ -28724,8 +29937,14 @@
       <c r="C25">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>2012</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>677</v>
       </c>
@@ -28735,8 +29954,14 @@
       <c r="C26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>2013</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>685</v>
       </c>
@@ -28746,8 +29971,14 @@
       <c r="C27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>2014</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>699</v>
       </c>
@@ -28757,8 +29988,14 @@
       <c r="C28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>2015</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>702</v>
       </c>
@@ -28768,8 +30005,14 @@
       <c r="C29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>2016</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>712</v>
       </c>
@@ -28780,7 +30023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>248</v>
       </c>
@@ -28791,7 +30034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>721</v>
       </c>
@@ -29501,5 +30744,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>